<commit_message>
saves all reports to a ledger, fixed mulithreading issue
</commit_message>
<xml_diff>
--- a/templates/example_sheet.xlsx
+++ b/templates/example_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\build\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C86B11-5AAA-4971-9318-12B80EEBFFA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89910365-69B8-4F93-BBE2-737DB9C95B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="0" windowWidth="19965" windowHeight="15600" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
+    <workbookView xWindow="5955" yWindow="0" windowWidth="22155" windowHeight="15600" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Equipment Name</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Ceiling</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Medical</t>
   </si>
 </sst>
 </file>
@@ -450,19 +456,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E901D-60E5-4378-B586-84E02EFBE42E}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,209 +477,224 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
         <v>335</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.121</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2.5</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1.5</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>75</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>30</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>20.5</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1.5</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>-1.5</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>74.25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
         <v>137</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.121</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2.5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1.5</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>75</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>30</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>21.5</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1.5</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>-3.5</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>24.5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
         <v>295</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.121</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2.5</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>75</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>64</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>28</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1.5</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>-3.5</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>39.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
         <v>400</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1.121</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>2.5</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>15</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>75</v>
-      </c>
-      <c r="L5">
-        <v>14</v>
       </c>
       <c r="M5">
         <v>14</v>
       </c>
       <c r="N5">
+        <v>14</v>
+      </c>
+      <c r="O5">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improved documentation, more information to the user
</commit_message>
<xml_diff>
--- a/templates/example_sheet.xlsx
+++ b/templates/example_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89910365-69B8-4F93-BBE2-737DB9C95B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303D6B26-4062-4636-8C48-70FFB096FC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5955" yWindow="0" windowWidth="22155" windowHeight="15600" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Equipment Name</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Medical</t>
+  </si>
+  <si>
+    <t>Medical, ICU</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +527,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>335</v>

</xml_diff>

<commit_message>
universal seperator now comma
</commit_message>
<xml_diff>
--- a/templates/example_sheet.xlsx
+++ b/templates/example_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303D6B26-4062-4636-8C48-70FFB096FC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49056985-2452-4801-94AD-89FBD96B1E6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5955" yWindow="0" windowWidth="22155" windowHeight="15600" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t xml:space="preserve">Anesthesia Machine </t>
   </si>
   <si>
-    <t>Wall+Floor</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Medical, ICU</t>
+  </si>
+  <si>
+    <t>Wall, Floor</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -504,19 +504,19 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -524,10 +524,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>335</v>
@@ -568,13 +568,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>137</v>
@@ -615,13 +615,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>295</v>
@@ -662,13 +662,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>400</v>

</xml_diff>

<commit_message>
user can now include units in the inputs
</commit_message>
<xml_diff>
--- a/templates/example_sheet.xlsx
+++ b/templates/example_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7340A7-B9F1-49E8-A6F8-7D904504EBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AEB385-B54A-4ACA-AB2D-E93639A0768E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6833" yWindow="978" windowWidth="26083" windowHeight="13925" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
+    <workbookView xWindow="6983" yWindow="978" windowWidth="25933" windowHeight="13925" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>tags</t>
   </si>
   <si>
-    <t>w_p_input</t>
-  </si>
-  <si>
     <t>s_ds_input</t>
   </si>
   <si>
@@ -95,22 +92,25 @@
     <t>h_input</t>
   </si>
   <si>
-    <t>capital_a_input</t>
-  </si>
-  <si>
-    <t>capital_b_input</t>
-  </si>
-  <si>
-    <t>a_input</t>
-  </si>
-  <si>
-    <t>b_input</t>
-  </si>
-  <si>
-    <t>capital_h_input</t>
-  </si>
-  <si>
     <t>omega_input</t>
+  </si>
+  <si>
+    <t>w_p_input(lb)</t>
+  </si>
+  <si>
+    <t>capital_a_input(in)</t>
+  </si>
+  <si>
+    <t>capital_b_input(in)</t>
+  </si>
+  <si>
+    <t>a_input(in)</t>
+  </si>
+  <si>
+    <t>b_input(in)</t>
+  </si>
+  <si>
+    <t>capital_h_input(ft)</t>
   </si>
 </sst>
 </file>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E901D-60E5-4378-B586-84E02EFBE42E}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -486,43 +486,43 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
         <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added preview images (only for mounting locations)
</commit_message>
<xml_diff>
--- a/templates/example_sheet.xlsx
+++ b/templates/example_sheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AEB385-B54A-4ACA-AB2D-E93639A0768E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A65ECD-E806-4D77-B133-B57F0D05A1FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6983" yWindow="978" windowWidth="25933" windowHeight="13925" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
+    <workbookView xWindow="20866" yWindow="992" windowWidth="13585" windowHeight="16913" activeTab="1" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
+    <sheet name="preview_images" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t xml:space="preserve">Anesthesia Machine </t>
   </si>
@@ -111,6 +112,24 @@
   </si>
   <si>
     <t>capital_h_input(ft)</t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>floor</t>
+  </si>
+  <si>
+    <t>wall,floor</t>
+  </si>
+  <si>
+    <t>Mounting Location</t>
+  </si>
+  <si>
+    <t>Preview image</t>
+  </si>
+  <si>
+    <t>ceiling</t>
   </si>
 </sst>
 </file>
@@ -163,6 +182,211 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>396815</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>301925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2835555</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1245032</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CFBE952-20C1-4A68-BB31-70113CFA3689}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1673524" y="483080"/>
+          <a:ext cx="2438740" cy="943107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>681487</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>577970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1996120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>835181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58E3CC9B-551B-41FE-AC43-A4CA33237C76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1958196" y="2475781"/>
+          <a:ext cx="1314633" cy="257211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1219370</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>476316</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8289E427-FCBC-4230-9505-EE1BFBB87CDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276709" y="3692106"/>
+          <a:ext cx="1219370" cy="476316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1257475</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142895</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{421968C0-7DF1-4F38-9A7B-5E258BA331BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276709" y="5512279"/>
+          <a:ext cx="1257475" cy="142895"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E901D-60E5-4378-B586-84E02EFBE42E}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -722,4 +946,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625FF69C-FFD7-4FF3-94D0-816D33E7369C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="56.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="135.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="141.30000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="143.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="171.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug that wasn't saving equipment names to reports
</commit_message>
<xml_diff>
--- a/templates/example_sheet.xlsx
+++ b/templates/example_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A65ECD-E806-4D77-B133-B57F0D05A1FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1402DF-1A75-40F8-BEF0-B4A95108F163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20866" yWindow="992" windowWidth="13585" windowHeight="16913" activeTab="1" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
+    <workbookView xWindow="68" yWindow="0" windowWidth="17606" windowHeight="16913" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
@@ -145,12 +145,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,8 +171,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E901D-60E5-4378-B586-84E02EFBE42E}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -697,16 +704,26 @@
     <col min="1" max="1" width="32.125" customWidth="1"/>
     <col min="2" max="2" width="25.125" customWidth="1"/>
     <col min="3" max="3" width="21.75" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="16.875" customWidth="1"/>
+    <col min="7" max="7" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="15.125" customWidth="1"/>
+    <col min="11" max="11" width="16.75" customWidth="1"/>
+    <col min="12" max="12" width="16.625" customWidth="1"/>
+    <col min="13" max="13" width="17.25" customWidth="1"/>
+    <col min="14" max="14" width="14.25" customWidth="1"/>
+    <col min="15" max="15" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
@@ -952,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625FF69C-FFD7-4FF3-94D0-816D33E7369C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>